<commit_message>
cap nhat project plan
</commit_message>
<xml_diff>
--- a/Project Plan Nhom2.xlsx
+++ b/Project Plan Nhom2.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Calculator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -126,7 +131,7 @@
     <t>Stt</t>
   </si>
   <si>
-    <t>in progress</t>
+    <t>skipped</t>
   </si>
 </sst>
 </file>
@@ -524,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -535,7 +540,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>